<commit_message>
Changes in Data source
</commit_message>
<xml_diff>
--- a/Rajupalem Land Records.xlsx
+++ b/Rajupalem Land Records.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhir\OneDrive\Desktop\Rajupalem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhir\OneDrive\Desktop\streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AF7DAC-412D-4D1D-9521-AA8FBDF24DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECB25DF-CD9F-4418-B764-5B7B351BB067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E098D626-A468-43A8-9D96-A4DF279CD8E2}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3310" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3314" uniqueCount="383">
   <si>
     <t>Account No.</t>
   </si>
@@ -1174,6 +1174,9 @@
   </si>
   <si>
     <t>Avula Srinivas Rao/ Lakshmi narayana</t>
+  </si>
+  <si>
+    <t>Avula Seshamma</t>
   </si>
 </sst>
 </file>
@@ -1235,15 +1238,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1562,8 +1562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F8FF5C-CF46-4217-96AB-43424F0C125D}">
   <dimension ref="A1:J1621"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
-      <selection activeCell="F222" sqref="F222"/>
+    <sheetView tabSelected="1" topLeftCell="C815" workbookViewId="0">
+      <selection activeCell="H827" sqref="H827"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14863,7 +14863,7 @@
       <c r="B475" s="1">
         <v>493</v>
       </c>
-      <c r="C475" s="3" t="s">
+      <c r="C475" s="1" t="s">
         <v>237</v>
       </c>
       <c r="D475" s="1">
@@ -14891,7 +14891,7 @@
       <c r="B476" s="1">
         <v>493</v>
       </c>
-      <c r="C476" s="3" t="s">
+      <c r="C476" s="1" t="s">
         <v>237</v>
       </c>
       <c r="D476" s="1">
@@ -14919,7 +14919,7 @@
       <c r="B477" s="1">
         <v>493</v>
       </c>
-      <c r="C477" s="3" t="s">
+      <c r="C477" s="1" t="s">
         <v>237</v>
       </c>
       <c r="D477" s="1">
@@ -14947,7 +14947,7 @@
       <c r="B478" s="1">
         <v>493</v>
       </c>
-      <c r="C478" s="3" t="s">
+      <c r="C478" s="1" t="s">
         <v>237</v>
       </c>
       <c r="D478" s="1">
@@ -14975,7 +14975,7 @@
       <c r="B479" s="1">
         <v>493</v>
       </c>
-      <c r="C479" s="3" t="s">
+      <c r="C479" s="1" t="s">
         <v>237</v>
       </c>
       <c r="D479" s="1">
@@ -24716,13 +24716,27 @@
       <c r="A827" s="1">
         <v>826</v>
       </c>
-      <c r="B827" s="1"/>
-      <c r="C827" s="1"/>
-      <c r="D827" s="1"/>
-      <c r="E827" s="1"/>
-      <c r="F827" s="1"/>
-      <c r="G827" s="1"/>
-      <c r="H827" s="1"/>
+      <c r="B827" s="1">
+        <v>802</v>
+      </c>
+      <c r="C827" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="D827" s="1">
+        <v>987</v>
+      </c>
+      <c r="E827" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F827" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G827" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H827" s="1">
+        <v>0.35</v>
+      </c>
       <c r="I827" s="1"/>
       <c r="J827" s="1"/>
     </row>

</xml_diff>

<commit_message>
Additions in data source
</commit_message>
<xml_diff>
--- a/Rajupalem Land Records.xlsx
+++ b/Rajupalem Land Records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhir\OneDrive\Desktop\streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECB25DF-CD9F-4418-B764-5B7B351BB067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1A1885-6693-4CC2-AE12-10ADA5231793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E098D626-A468-43A8-9D96-A4DF279CD8E2}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3314" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3318" uniqueCount="384">
   <si>
     <t>Account No.</t>
   </si>
@@ -1177,6 +1177,9 @@
   </si>
   <si>
     <t>Avula Seshamma</t>
+  </si>
+  <si>
+    <t>Eerla Edukondalu</t>
   </si>
 </sst>
 </file>
@@ -1562,8 +1565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F8FF5C-CF46-4217-96AB-43424F0C125D}">
   <dimension ref="A1:J1621"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C815" workbookViewId="0">
-      <selection activeCell="H827" sqref="H827"/>
+    <sheetView tabSelected="1" topLeftCell="A819" workbookViewId="0">
+      <selection activeCell="C800" sqref="C800"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24744,13 +24747,27 @@
       <c r="A828" s="1">
         <v>827</v>
       </c>
-      <c r="B828" s="1"/>
-      <c r="C828" s="1"/>
-      <c r="D828" s="1"/>
-      <c r="E828" s="1"/>
-      <c r="F828" s="1"/>
-      <c r="G828" s="1"/>
-      <c r="H828" s="1"/>
+      <c r="B828" s="1">
+        <v>803</v>
+      </c>
+      <c r="C828" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D828" s="1">
+        <v>937</v>
+      </c>
+      <c r="E828" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F828" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G828" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H828" s="1">
+        <v>0.1</v>
+      </c>
       <c r="I828" s="1"/>
       <c r="J828" s="1"/>
     </row>

</xml_diff>